<commit_message>
processing GCOOS. creating inventory from processed files only.
</commit_message>
<xml_diff>
--- a/2020/data/processed/AOOS.xlsx
+++ b/2020/data/processed/AOOS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="569">
   <si>
     <t>Station ID</t>
   </si>
@@ -1655,9 +1655,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>Something newly added or changed to spreadsheet</t>
-  </si>
-  <si>
     <t>Found it on AOOS portal, reporting since 2018, was offline a bit in early 2019, but reporting otherwise.</t>
   </si>
   <si>
@@ -1853,9 +1850,6 @@
     <t>Stopped reportng July 2020.</t>
   </si>
   <si>
-    <t>Removed (I could not use the strike out feature), so grey shaded and moved a copy to the Not Reportingin 2020 worksheet.</t>
-  </si>
-  <si>
     <t>NREL Kodiak, AK CDIP Wave Buoy 236</t>
   </si>
   <si>
@@ -1931,9 +1925,6 @@
     <t>PWSRCAC, MicroSspecialties (private industry)</t>
   </si>
   <si>
-    <t>NOTE 2020</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -2022,9 +2013,6 @@
   </si>
   <si>
     <t>Hoping this comes online in 2021</t>
-  </si>
-  <si>
-    <t>Some of the station start dates changed in the data portal records, so I reflect those changes on this version of the AI for the MXAK AIS WX stations. The dates highlighted in Yellow, and some of those may not reflect the actual install dates. I leave two dates on some, so I can reference with MXAK. I believe the portal start dates arer of intitialized data on the data portal. I will need to confer with MXAK to determine actual install dates, if needed. I am not sure they stored their data, so it might only be useful to know when a perm record was being made. Only the NDBC station feeds will have historical records  if we we do not already host them. This needs investigation.</t>
   </si>
   <si>
     <t>Need to check install date (2014) vs date AOOS started reporting (July 2017)</t>
@@ -2285,7 +2273,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2419,9 +2407,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2919,12 +2904,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3123,7 +3108,7 @@
         <v>396</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>392</v>
@@ -3276,7 +3261,7 @@
       <c r="Q6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R6" s="65"/>
+      <c r="R6" s="64"/>
       <c r="S6" s="42"/>
     </row>
     <row r="7" spans="1:20" ht="28.8">
@@ -3328,7 +3313,7 @@
       <c r="Q7" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="R7" s="65"/>
+      <c r="R7" s="64"/>
       <c r="S7" s="42"/>
     </row>
     <row r="8" spans="1:20" s="32" customFormat="1" ht="28.8">
@@ -3353,7 +3338,7 @@
       <c r="H8" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="53">
         <v>42900</v>
       </c>
       <c r="J8" s="31" t="s">
@@ -3437,24 +3422,24 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:20" s="50" customFormat="1" ht="28.8">
+    <row r="10" spans="1:20" s="49" customFormat="1" ht="28.8">
       <c r="A10" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="40" t="s">
+        <v>495</v>
+      </c>
+      <c r="E10" s="40" t="s">
         <v>496</v>
       </c>
-      <c r="E10" s="40" t="s">
-        <v>497</v>
-      </c>
-      <c r="F10" s="78">
+      <c r="F10" s="77">
         <v>60.791499999999999</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="77">
         <v>-161.74870000000001</v>
       </c>
       <c r="H10" s="40" t="s">
@@ -3488,7 +3473,7 @@
         <v>314</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="S10" s="47"/>
     </row>
@@ -3545,7 +3530,7 @@
         <v>314</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -3556,8 +3541,8 @@
       <c r="B12" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="D12" s="64" t="s">
-        <v>470</v>
+      <c r="D12" s="63" t="s">
+        <v>469</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>288</v>
@@ -3571,7 +3556,7 @@
       <c r="H12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="53">
+      <c r="I12" s="52">
         <v>43446</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -3672,7 +3657,7 @@
       <c r="H14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="60">
+      <c r="I14" s="59">
         <v>42278</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -3724,7 +3709,7 @@
       <c r="H15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I15" s="59">
         <v>42129</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -3755,27 +3740,27 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" s="50" customFormat="1" ht="28.8">
+    <row r="16" spans="1:20" s="49" customFormat="1" ht="28.8">
       <c r="A16" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="46" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="65">
         <v>53.889099999999999</v>
       </c>
-      <c r="G16" s="66">
+      <c r="G16" s="65">
         <v>-166.54212000000001</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="71" t="s">
         <v>84</v>
       </c>
       <c r="I16" s="48">
@@ -3802,11 +3787,11 @@
       <c r="P16" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="98" t="s">
-        <v>492</v>
+      <c r="Q16" s="97" t="s">
+        <v>491</v>
       </c>
       <c r="R16" s="46" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="28.8">
@@ -3831,7 +3816,7 @@
       <c r="H17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I17" s="60">
+      <c r="I17" s="59">
         <v>42187</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -3937,7 +3922,7 @@
       <c r="G19" s="29">
         <v>-171.71530999999999</v>
       </c>
-      <c r="H19" s="102" t="s">
+      <c r="H19" s="101" t="s">
         <v>84</v>
       </c>
       <c r="I19" s="2">
@@ -3968,24 +3953,24 @@
         <v>314</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="50" customFormat="1" ht="28.8">
+    <row r="20" spans="1:20" s="49" customFormat="1" ht="28.8">
       <c r="A20" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40" t="s">
-        <v>499</v>
-      </c>
-      <c r="E20" s="73" t="s">
-        <v>550</v>
-      </c>
-      <c r="F20" s="78">
+        <v>498</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>547</v>
+      </c>
+      <c r="F20" s="77">
         <v>58.211799999999997</v>
       </c>
-      <c r="G20" s="78">
+      <c r="G20" s="77">
         <v>-136.38130000000001</v>
       </c>
       <c r="H20" s="40" t="s">
@@ -4003,23 +3988,23 @@
       <c r="L20" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="103" t="s">
+      <c r="M20" s="102" t="s">
         <v>286</v>
       </c>
-      <c r="N20" s="103" t="s">
+      <c r="N20" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="O20" s="103" t="s">
+      <c r="O20" s="102" t="s">
         <v>86</v>
       </c>
       <c r="P20" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="Q20" s="104" t="s">
+      <c r="Q20" s="103" t="s">
         <v>314</v>
       </c>
       <c r="R20" s="40" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="S20" s="47"/>
     </row>
@@ -4103,7 +4088,7 @@
       <c r="H22" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="54">
+      <c r="I22" s="53">
         <v>41901</v>
       </c>
       <c r="J22" s="31" t="s">
@@ -4131,7 +4116,7 @@
         <v>314</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="S22" s="35"/>
     </row>
@@ -4160,7 +4145,7 @@
       <c r="H23" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="54">
+      <c r="I23" s="53">
         <v>42248</v>
       </c>
       <c r="J23" s="31" t="s">
@@ -4387,7 +4372,7 @@
       <c r="H27" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="54">
+      <c r="I27" s="53">
         <v>42942</v>
       </c>
       <c r="J27" s="31" t="s">
@@ -4441,7 +4426,7 @@
       <c r="H28" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="54">
+      <c r="I28" s="53">
         <v>42942</v>
       </c>
       <c r="J28" s="31" t="s">
@@ -4498,7 +4483,7 @@
       <c r="H29" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="54">
+      <c r="I29" s="53">
         <v>42942</v>
       </c>
       <c r="J29" s="31" t="s">
@@ -4552,7 +4537,7 @@
       <c r="H30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="60">
+      <c r="I30" s="59">
         <v>43313</v>
       </c>
       <c r="J30" s="3" t="s">
@@ -4580,7 +4565,7 @@
         <v>314</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="28.8">
@@ -4710,12 +4695,12 @@
         <v>55.339500000000001</v>
       </c>
       <c r="G33" s="31">
-        <v>-1331.644231</v>
+        <v>-131.64423099999999</v>
       </c>
       <c r="H33" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="53">
         <v>42944</v>
       </c>
       <c r="J33" s="31" t="s">
@@ -4769,7 +4754,7 @@
       <c r="H34" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="I34" s="59">
+      <c r="I34" s="58">
         <v>42514</v>
       </c>
       <c r="J34" s="1" t="s">
@@ -4879,7 +4864,7 @@
       <c r="H36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I36" s="63">
+      <c r="I36" s="62">
         <v>42139</v>
       </c>
       <c r="J36" s="1" t="s">
@@ -5318,7 +5303,7 @@
       <c r="H44" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I44" s="54">
+      <c r="I44" s="53">
         <v>42942</v>
       </c>
       <c r="J44" s="31" t="s">
@@ -5375,7 +5360,7 @@
       <c r="H45" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I45" s="54">
+      <c r="I45" s="53">
         <v>42877</v>
       </c>
       <c r="J45" s="31" t="s">
@@ -5471,7 +5456,7 @@
       <c r="B47" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="C47" s="99" t="s">
+      <c r="C47" s="98" t="s">
         <v>371</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -5489,7 +5474,7 @@
       <c r="H47" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I47" s="100">
+      <c r="I47" s="99">
         <v>43446</v>
       </c>
       <c r="J47" s="3" t="s">
@@ -5514,10 +5499,10 @@
         <v>283</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="28.8">
@@ -5527,7 +5512,7 @@
       <c r="B48" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="101" t="s">
+      <c r="C48" s="100" t="s">
         <v>369</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5595,7 +5580,7 @@
       <c r="G49" s="29">
         <v>-170.492243</v>
       </c>
-      <c r="H49" s="102" t="s">
+      <c r="H49" s="101" t="s">
         <v>84</v>
       </c>
       <c r="I49" s="2">
@@ -5706,7 +5691,7 @@
       <c r="H51" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I51" s="54">
+      <c r="I51" s="53">
         <v>42527</v>
       </c>
       <c r="J51" s="31" t="s">
@@ -5738,27 +5723,27 @@
       </c>
       <c r="S51" s="35"/>
     </row>
-    <row r="52" spans="1:20" s="50" customFormat="1" ht="28.8">
+    <row r="52" spans="1:20" s="49" customFormat="1" ht="28.8">
       <c r="A52" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C52" s="46"/>
       <c r="D52" s="46" t="s">
-        <v>472</v>
-      </c>
-      <c r="E52" s="73" t="s">
-        <v>550</v>
-      </c>
-      <c r="F52" s="66">
+        <v>471</v>
+      </c>
+      <c r="E52" s="72" t="s">
+        <v>547</v>
+      </c>
+      <c r="F52" s="65">
         <v>53.5989</v>
       </c>
-      <c r="G52" s="66">
+      <c r="G52" s="65">
         <v>-132.20320000000001</v>
       </c>
-      <c r="H52" s="72" t="s">
+      <c r="H52" s="71" t="s">
         <v>84</v>
       </c>
       <c r="I52" s="48">
@@ -5785,11 +5770,11 @@
       <c r="P52" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="Q52" s="98" t="s">
+      <c r="Q52" s="97" t="s">
+        <v>491</v>
+      </c>
+      <c r="R52" s="46" t="s">
         <v>492</v>
-      </c>
-      <c r="R52" s="46" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="53" spans="1:20" s="32" customFormat="1" ht="28.8">
@@ -5817,7 +5802,7 @@
       <c r="H53" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I53" s="54">
+      <c r="I53" s="53">
         <v>42468</v>
       </c>
       <c r="J53" s="31" t="s">
@@ -5874,7 +5859,7 @@
       <c r="H54" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I54" s="54">
+      <c r="I54" s="53">
         <v>42487</v>
       </c>
       <c r="J54" s="31" t="s">
@@ -5931,7 +5916,7 @@
       <c r="H55" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I55" s="54">
+      <c r="I55" s="53">
         <v>42402</v>
       </c>
       <c r="J55" s="31" t="s">
@@ -6020,58 +6005,58 @@
       </c>
       <c r="S56" s="1"/>
     </row>
-    <row r="57" spans="1:20" s="80" customFormat="1" ht="28.8">
-      <c r="A57" s="80" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="79" t="s">
+    <row r="57" spans="1:20" s="79" customFormat="1" ht="28.8">
+      <c r="A57" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="78" t="s">
+        <v>502</v>
+      </c>
+      <c r="C57" s="80"/>
+      <c r="D57" s="78" t="s">
         <v>503</v>
       </c>
-      <c r="C57" s="81"/>
-      <c r="D57" s="79" t="s">
-        <v>504</v>
-      </c>
-      <c r="E57" s="73" t="s">
+      <c r="E57" s="72" t="s">
         <v>400</v>
       </c>
-      <c r="F57" s="80">
+      <c r="F57" s="79">
         <v>54.802599999999998</v>
       </c>
-      <c r="G57" s="80">
+      <c r="G57" s="79">
         <v>-130.93440000000001</v>
       </c>
-      <c r="H57" s="79" t="s">
+      <c r="H57" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="I57" s="54">
+      <c r="I57" s="53">
         <v>43821</v>
       </c>
-      <c r="J57" s="79" t="s">
+      <c r="J57" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="K57" s="79" t="s">
+      <c r="K57" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="L57" s="79" t="s">
+      <c r="L57" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="M57" s="79" t="s">
+      <c r="M57" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="N57" s="79" t="s">
+      <c r="N57" s="78" t="s">
         <v>38</v>
       </c>
       <c r="O57" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="P57" s="79"/>
+      <c r="P57" s="78"/>
       <c r="Q57" s="47" t="s">
         <v>314</v>
       </c>
-      <c r="R57" s="79" t="s">
-        <v>505</v>
-      </c>
-      <c r="S57" s="82"/>
+      <c r="R57" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="S57" s="81"/>
     </row>
     <row r="58" spans="1:20" ht="28.8">
       <c r="A58" s="10" t="s">
@@ -6095,7 +6080,7 @@
       <c r="H58" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="63">
+      <c r="I58" s="62">
         <v>42129</v>
       </c>
       <c r="J58" s="23" t="s">
@@ -6147,7 +6132,7 @@
       <c r="H59" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I59" s="60">
+      <c r="I59" s="59">
         <v>42942</v>
       </c>
       <c r="J59" s="1" t="s">
@@ -6197,7 +6182,7 @@
       <c r="H60" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I60" s="60">
+      <c r="I60" s="59">
         <v>43313</v>
       </c>
       <c r="J60" s="3" t="s">
@@ -6248,8 +6233,8 @@
       <c r="H61" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I61" s="60" t="s">
-        <v>506</v>
+      <c r="I61" s="59" t="s">
+        <v>505</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>35</v>
@@ -6300,7 +6285,7 @@
       <c r="H62" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I62" s="54">
+      <c r="I62" s="53">
         <v>42864</v>
       </c>
       <c r="J62" s="31" t="s">
@@ -6341,7 +6326,7 @@
         <v>46108</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>312</v>
@@ -6398,7 +6383,7 @@
         <v>46264</v>
       </c>
       <c r="D64" s="46" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>310</v>
@@ -6437,10 +6422,10 @@
         <v>40</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="R64" s="40" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="65" spans="1:20" s="19" customFormat="1" ht="125.25" customHeight="1">
@@ -6454,10 +6439,10 @@
         <v>46265</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F65" s="1">
         <v>64.472300000000004</v>
@@ -6472,7 +6457,7 @@
         <v>43297</v>
       </c>
       <c r="J65" s="40" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K65" s="23" t="s">
         <v>405</v>
@@ -6493,10 +6478,10 @@
         <v>40</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="R65" s="40" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="S65" s="3"/>
       <c r="T65" s="5"/>
@@ -6523,7 +6508,7 @@
       <c r="H66" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I66" s="59">
+      <c r="I66" s="58">
         <v>42129</v>
       </c>
       <c r="J66" s="5" t="s">
@@ -6631,7 +6616,7 @@
       <c r="H68" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I68" s="59">
+      <c r="I68" s="58">
         <v>42129</v>
       </c>
       <c r="J68" s="5" t="s">
@@ -6779,7 +6764,7 @@
         <v>185</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>186</v>
@@ -6833,7 +6818,7 @@
         <v>308</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>192</v>
@@ -6875,24 +6860,24 @@
         <v>346</v>
       </c>
       <c r="R72" s="40" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="S72" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="73" spans="1:20" s="50" customFormat="1" ht="43.2">
+    <row r="73" spans="1:20" s="49" customFormat="1" ht="43.2">
       <c r="A73" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="64" t="s">
-        <v>520</v>
+      <c r="B73" s="63" t="s">
+        <v>518</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E73" s="40" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F73" s="47">
         <v>50.116</v>
@@ -6910,7 +6895,7 @@
         <v>35</v>
       </c>
       <c r="K73" s="40" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="L73" s="40" t="s">
         <v>77</v>
@@ -6919,7 +6904,7 @@
         <v>199</v>
       </c>
       <c r="N73" s="40" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="O73" s="40" t="s">
         <v>199</v>
@@ -6931,9 +6916,9 @@
         <v>346</v>
       </c>
       <c r="R73" s="40" t="s">
-        <v>527</v>
-      </c>
-      <c r="S73" s="106"/>
+        <v>525</v>
+      </c>
+      <c r="S73" s="105"/>
     </row>
     <row r="74" spans="1:20" ht="28.8">
       <c r="A74" s="10" t="s">
@@ -6991,61 +6976,61 @@
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="1:20" s="55" customFormat="1" ht="100.05" customHeight="1">
-      <c r="A75" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="B75" s="69" t="s">
+    <row r="75" spans="1:20" s="54" customFormat="1" ht="100.05" customHeight="1">
+      <c r="A75" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="C75" s="73"/>
+      <c r="C75" s="72"/>
       <c r="D75" s="41" t="s">
-        <v>528</v>
-      </c>
-      <c r="E75" s="65" t="s">
-        <v>466</v>
-      </c>
-      <c r="F75" s="58">
+        <v>526</v>
+      </c>
+      <c r="E75" s="64" t="s">
+        <v>465</v>
+      </c>
+      <c r="F75" s="57">
         <v>66.895034999999993</v>
       </c>
-      <c r="G75" s="58">
+      <c r="G75" s="57">
         <v>-162.56675000000001</v>
       </c>
-      <c r="H75" s="65" t="s">
+      <c r="H75" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="I75" s="57">
+      <c r="I75" s="56">
         <v>43348</v>
       </c>
-      <c r="J75" s="65" t="s">
+      <c r="J75" s="64" t="s">
         <v>443</v>
       </c>
-      <c r="K75" s="65" t="s">
+      <c r="K75" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="L75" s="65" t="s">
+      <c r="L75" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="M75" s="65" t="s">
+      <c r="M75" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="N75" s="65" t="s">
+      <c r="N75" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="O75" s="107" t="s">
+      <c r="O75" s="106" t="s">
         <v>207</v>
       </c>
-      <c r="P75" s="65" t="s">
+      <c r="P75" s="64" t="s">
         <v>416</v>
       </c>
-      <c r="Q75" s="108" t="s">
+      <c r="Q75" s="107" t="s">
         <v>338</v>
       </c>
-      <c r="R75" s="65" t="s">
-        <v>468</v>
-      </c>
-      <c r="S75" s="55" t="s">
-        <v>507</v>
+      <c r="R75" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="S75" s="54" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="28.8">
@@ -7059,10 +7044,10 @@
         <v>373</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F76" s="1">
         <v>66.926820000000006</v>
@@ -7104,7 +7089,7 @@
         <v>208</v>
       </c>
       <c r="S76" s="19" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T76" s="19"/>
     </row>
@@ -7770,452 +7755,452 @@
       <c r="S88" s="1"/>
     </row>
     <row r="89" spans="1:19" ht="28.8">
-      <c r="A89" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="B89" s="55" t="s">
+      <c r="A89" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B89" s="54" t="s">
+        <v>446</v>
+      </c>
+      <c r="C89" s="66"/>
+      <c r="D89" s="66" t="s">
         <v>447</v>
       </c>
-      <c r="C89" s="67"/>
-      <c r="D89" s="67" t="s">
+      <c r="E89" s="66" t="s">
+        <v>348</v>
+      </c>
+      <c r="F89" s="55">
+        <v>70.204099999999997</v>
+      </c>
+      <c r="G89" s="55">
+        <v>-147.70140000000001</v>
+      </c>
+      <c r="H89" s="67" t="s">
         <v>448</v>
       </c>
-      <c r="E89" s="67" t="s">
-        <v>348</v>
-      </c>
-      <c r="F89" s="56">
-        <v>70.204099999999997</v>
-      </c>
-      <c r="G89" s="56">
-        <v>-147.70140000000001</v>
-      </c>
-      <c r="H89" s="68" t="s">
-        <v>449</v>
-      </c>
-      <c r="I89" s="57">
+      <c r="I89" s="56">
         <v>43307</v>
       </c>
       <c r="J89" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="K89" s="65" t="s">
+      <c r="K89" s="64" t="s">
         <v>266</v>
       </c>
-      <c r="L89" s="67" t="s">
+      <c r="L89" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="M89" s="67" t="s">
+      <c r="M89" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="N89" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="O89" s="66" t="s">
         <v>450</v>
       </c>
-      <c r="N89" s="67" t="s">
+      <c r="P89" s="66" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q89" s="57" t="s">
+        <v>314</v>
+      </c>
+      <c r="R89" s="72" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="57.6">
+      <c r="A90" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B90" s="54" t="s">
+        <v>453</v>
+      </c>
+      <c r="C90" s="66"/>
+      <c r="D90" s="66" t="s">
+        <v>463</v>
+      </c>
+      <c r="E90" s="76" t="s">
+        <v>528</v>
+      </c>
+      <c r="F90" s="55">
+        <v>70.319000000000003</v>
+      </c>
+      <c r="G90" s="55">
+        <v>-147.7612</v>
+      </c>
+      <c r="H90" s="67" t="s">
+        <v>454</v>
+      </c>
+      <c r="I90" s="56">
+        <v>43683</v>
+      </c>
+      <c r="J90" s="41" t="s">
+        <v>530</v>
+      </c>
+      <c r="K90" s="64" t="s">
+        <v>266</v>
+      </c>
+      <c r="L90" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="M90" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="N90" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="O89" s="67" t="s">
+      <c r="O90" s="66" t="s">
+        <v>450</v>
+      </c>
+      <c r="P90" s="66" t="s">
         <v>451</v>
       </c>
-      <c r="P89" s="67" t="s">
-        <v>452</v>
-      </c>
-      <c r="Q89" s="58" t="s">
-        <v>314</v>
-      </c>
-      <c r="R89" s="73" t="s">
+      <c r="Q90" s="66" t="s">
+        <v>455</v>
+      </c>
+      <c r="R90" s="72" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="57.6">
-      <c r="A90" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="B90" s="55" t="s">
+    <row r="91" spans="1:19" ht="57.6">
+      <c r="A91" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="54" t="s">
+        <v>456</v>
+      </c>
+      <c r="C91" s="66"/>
+      <c r="D91" s="66" t="s">
+        <v>464</v>
+      </c>
+      <c r="E91" s="76" t="s">
+        <v>528</v>
+      </c>
+      <c r="F91" s="55">
+        <v>70.393500000000003</v>
+      </c>
+      <c r="G91" s="55">
+        <v>-147.83500000000001</v>
+      </c>
+      <c r="H91" s="67" t="s">
         <v>454</v>
       </c>
-      <c r="C90" s="67"/>
-      <c r="D90" s="67" t="s">
-        <v>464</v>
-      </c>
-      <c r="E90" s="77" t="s">
+      <c r="I91" s="56">
+        <v>43684</v>
+      </c>
+      <c r="J91" s="41" t="s">
         <v>530</v>
       </c>
-      <c r="F90" s="56">
-        <v>70.319000000000003</v>
-      </c>
-      <c r="G90" s="56">
-        <v>-147.7612</v>
-      </c>
-      <c r="H90" s="68" t="s">
+      <c r="K91" s="64" t="s">
+        <v>266</v>
+      </c>
+      <c r="L91" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="M91" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="N91" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="O91" s="66" t="s">
+        <v>450</v>
+      </c>
+      <c r="P91" s="66" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q91" s="66" t="s">
         <v>455</v>
       </c>
-      <c r="I90" s="57">
-        <v>43683</v>
-      </c>
-      <c r="J90" s="41" t="s">
-        <v>532</v>
-      </c>
-      <c r="K90" s="65" t="s">
-        <v>266</v>
-      </c>
-      <c r="L90" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="M90" s="67" t="s">
-        <v>450</v>
-      </c>
-      <c r="N90" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="O90" s="67" t="s">
-        <v>451</v>
-      </c>
-      <c r="P90" s="67" t="s">
-        <v>452</v>
-      </c>
-      <c r="Q90" s="67" t="s">
-        <v>456</v>
-      </c>
-      <c r="R90" s="73" t="s">
+      <c r="R91" s="72" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="57.6">
-      <c r="A91" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="B91" s="55" t="s">
-        <v>457</v>
-      </c>
-      <c r="C91" s="67"/>
-      <c r="D91" s="67" t="s">
-        <v>465</v>
-      </c>
-      <c r="E91" s="77" t="s">
-        <v>530</v>
-      </c>
-      <c r="F91" s="56">
-        <v>70.393500000000003</v>
-      </c>
-      <c r="G91" s="56">
-        <v>-147.83500000000001</v>
-      </c>
-      <c r="H91" s="68" t="s">
-        <v>455</v>
-      </c>
-      <c r="I91" s="57">
-        <v>43684</v>
-      </c>
-      <c r="J91" s="41" t="s">
-        <v>532</v>
-      </c>
-      <c r="K91" s="65" t="s">
-        <v>266</v>
-      </c>
-      <c r="L91" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="M91" s="67" t="s">
-        <v>450</v>
-      </c>
-      <c r="N91" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="O91" s="67" t="s">
-        <v>451</v>
-      </c>
-      <c r="P91" s="67" t="s">
-        <v>452</v>
-      </c>
-      <c r="Q91" s="67" t="s">
-        <v>456</v>
-      </c>
-      <c r="R91" s="73" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" s="77" customFormat="1" ht="43.2">
-      <c r="A92" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="B92" s="73" t="s">
+    <row r="92" spans="1:19" s="76" customFormat="1" ht="43.2">
+      <c r="A92" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" s="72" t="s">
+        <v>476</v>
+      </c>
+      <c r="D92" s="72" t="s">
         <v>477</v>
       </c>
-      <c r="D92" s="73" t="s">
-        <v>478</v>
-      </c>
-      <c r="E92" s="73" t="s">
-        <v>488</v>
-      </c>
-      <c r="F92" s="74">
+      <c r="E92" s="72" t="s">
+        <v>487</v>
+      </c>
+      <c r="F92" s="73">
         <v>59.798299999999998</v>
       </c>
-      <c r="G92" s="74">
+      <c r="G92" s="73">
         <v>-144.59989999999999</v>
       </c>
-      <c r="H92" s="75" t="s">
+      <c r="H92" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="I92" s="76">
+      <c r="I92" s="75">
         <v>41976</v>
       </c>
       <c r="J92" s="41" t="s">
         <v>35</v>
       </c>
       <c r="K92" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="L92" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="M92" s="72" t="s">
         <v>479</v>
       </c>
-      <c r="L92" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="M92" s="73" t="s">
+      <c r="N92" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="O92" s="72" t="s">
+        <v>533</v>
+      </c>
+      <c r="P92" s="72" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q92" s="72" t="s">
         <v>480</v>
       </c>
-      <c r="N92" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="O92" s="73" t="s">
-        <v>535</v>
-      </c>
-      <c r="P92" s="73" t="s">
-        <v>534</v>
-      </c>
-      <c r="Q92" s="73" t="s">
+    </row>
+    <row r="93" spans="1:19" s="76" customFormat="1" ht="100.8">
+      <c r="A93" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" s="72" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" s="77" customFormat="1" ht="100.8">
-      <c r="A93" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="B93" s="73" t="s">
+      <c r="D93" s="72" t="s">
         <v>482</v>
       </c>
-      <c r="D93" s="73" t="s">
-        <v>483</v>
-      </c>
-      <c r="E93" s="73" t="s">
-        <v>487</v>
-      </c>
-      <c r="F93" s="74">
+      <c r="E93" s="72" t="s">
+        <v>486</v>
+      </c>
+      <c r="F93" s="73">
         <v>61.091000000000001</v>
       </c>
-      <c r="G93" s="74">
+      <c r="G93" s="73">
         <v>-146.3766</v>
       </c>
-      <c r="H93" s="75" t="s">
-        <v>489</v>
-      </c>
-      <c r="I93" s="76">
+      <c r="H93" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="I93" s="75">
         <v>43729</v>
       </c>
       <c r="J93" s="41" t="s">
         <v>35</v>
       </c>
       <c r="K93" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="L93" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="M93" s="72" t="s">
         <v>479</v>
       </c>
-      <c r="L93" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="M93" s="73" t="s">
-        <v>480</v>
-      </c>
-      <c r="N93" s="73" t="s">
+      <c r="N93" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="O93" s="73" t="s">
+      <c r="O93" s="72" t="s">
+        <v>489</v>
+      </c>
+      <c r="P93" s="72" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q93" s="72" t="s">
         <v>490</v>
       </c>
-      <c r="P93" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q93" s="73" t="s">
-        <v>491</v>
-      </c>
-      <c r="R93" s="73" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" s="77" customFormat="1" ht="100.8">
-      <c r="A94" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="B94" s="73" t="s">
+      <c r="R93" s="72" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" s="76" customFormat="1" ht="100.8">
+      <c r="A94" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94" s="72" t="s">
+        <v>484</v>
+      </c>
+      <c r="D94" s="72" t="s">
         <v>485</v>
       </c>
-      <c r="D94" s="73" t="s">
+      <c r="E94" s="72" t="s">
         <v>486</v>
       </c>
-      <c r="E94" s="73" t="s">
-        <v>487</v>
-      </c>
-      <c r="F94" s="74">
+      <c r="F94" s="73">
         <v>61.122500000000002</v>
       </c>
-      <c r="G94" s="74">
+      <c r="G94" s="73">
         <v>-146.29669999999999</v>
       </c>
-      <c r="H94" s="75" t="s">
-        <v>489</v>
-      </c>
-      <c r="I94" s="76">
+      <c r="H94" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="I94" s="75">
         <v>43729</v>
       </c>
       <c r="J94" s="41" t="s">
         <v>35</v>
       </c>
       <c r="K94" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="L94" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="M94" s="72" t="s">
         <v>479</v>
       </c>
-      <c r="L94" s="73" t="s">
+      <c r="N94" s="72" t="s">
+        <v>483</v>
+      </c>
+      <c r="O94" s="72" t="s">
+        <v>489</v>
+      </c>
+      <c r="P94" s="72" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q94" s="72" t="s">
+        <v>490</v>
+      </c>
+      <c r="R94" s="72" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" s="108" customFormat="1">
+      <c r="A95" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" s="108" t="s">
+        <v>548</v>
+      </c>
+      <c r="D95" s="108" t="s">
+        <v>539</v>
+      </c>
+      <c r="E95" s="108" t="s">
+        <v>549</v>
+      </c>
+      <c r="F95" s="111">
+        <v>56.004100000000001</v>
+      </c>
+      <c r="G95" s="111">
+        <v>-161.17509999999999</v>
+      </c>
+      <c r="H95" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="I95" s="110">
+        <v>43586</v>
+      </c>
+      <c r="J95" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="K95" s="109" t="s">
+        <v>540</v>
+      </c>
+      <c r="L95" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="M94" s="73" t="s">
-        <v>480</v>
-      </c>
-      <c r="N94" s="73" t="s">
-        <v>484</v>
-      </c>
-      <c r="O94" s="73" t="s">
-        <v>490</v>
-      </c>
-      <c r="P94" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q94" s="73" t="s">
-        <v>491</v>
-      </c>
-      <c r="R94" s="73" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" s="109" customFormat="1">
-      <c r="A95" s="109" t="s">
-        <v>37</v>
-      </c>
-      <c r="B95" s="109" t="s">
-        <v>551</v>
-      </c>
-      <c r="D95" s="109" t="s">
-        <v>542</v>
-      </c>
-      <c r="E95" s="109" t="s">
+      <c r="M95" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="N95" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="O95" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="P95" s="109" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q95" s="108" t="s">
+        <v>414</v>
+      </c>
+      <c r="R95" s="109"/>
+    </row>
+    <row r="96" spans="1:19" ht="72">
+      <c r="A96" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" s="96" t="s">
         <v>552</v>
       </c>
-      <c r="F95" s="112">
-        <v>56.004100000000001</v>
-      </c>
-      <c r="G95" s="112">
-        <v>-161.17509999999999</v>
-      </c>
-      <c r="H95" s="109" t="s">
+      <c r="C96" s="96"/>
+      <c r="D96" s="96" t="s">
+        <v>543</v>
+      </c>
+      <c r="E96" s="96" t="s">
+        <v>553</v>
+      </c>
+      <c r="F96" s="122">
+        <v>58.732100000000003</v>
+      </c>
+      <c r="G96" s="122">
+        <v>-156.98330000000001</v>
+      </c>
+      <c r="H96" s="123" t="s">
         <v>84</v>
       </c>
-      <c r="I95" s="111">
-        <v>43586</v>
-      </c>
-      <c r="J95" s="109" t="s">
+      <c r="I96" s="124">
+        <v>43661</v>
+      </c>
+      <c r="J96" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="K95" s="110" t="s">
-        <v>543</v>
-      </c>
-      <c r="L95" s="109" t="s">
-        <v>77</v>
-      </c>
-      <c r="M95" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="N95" s="109" t="s">
-        <v>206</v>
-      </c>
-      <c r="O95" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="P95" s="110" t="s">
-        <v>553</v>
-      </c>
-      <c r="Q95" s="109" t="s">
+      <c r="K96" s="125" t="s">
+        <v>37</v>
+      </c>
+      <c r="L96" s="96" t="s">
+        <v>58</v>
+      </c>
+      <c r="M96" s="96" t="s">
+        <v>544</v>
+      </c>
+      <c r="N96" s="96" t="s">
+        <v>545</v>
+      </c>
+      <c r="O96" s="96" t="s">
+        <v>544</v>
+      </c>
+      <c r="P96" s="96" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q96" s="96" t="s">
         <v>414</v>
       </c>
-      <c r="R95" s="110"/>
-    </row>
-    <row r="96" spans="1:19" ht="72">
-      <c r="A96" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="B96" s="97" t="s">
+      <c r="R96" s="96" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="54" customFormat="1" ht="28.8">
+      <c r="A97" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B97" s="72" t="s">
+        <v>554</v>
+      </c>
+      <c r="C97" s="72"/>
+      <c r="D97" s="72" t="s">
+        <v>556</v>
+      </c>
+      <c r="E97" s="72" t="s">
         <v>555</v>
       </c>
-      <c r="C96" s="97"/>
-      <c r="D96" s="97" t="s">
-        <v>546</v>
-      </c>
-      <c r="E96" s="97" t="s">
-        <v>556</v>
-      </c>
-      <c r="F96" s="123">
-        <v>58.732100000000003</v>
-      </c>
-      <c r="G96" s="123">
-        <v>-156.98330000000001</v>
-      </c>
-      <c r="H96" s="124" t="s">
+      <c r="F97" s="73">
+        <v>59.605499999999999</v>
+      </c>
+      <c r="G97" s="73">
+        <v>-151.4221</v>
+      </c>
+      <c r="H97" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="I96" s="125">
-        <v>43661</v>
-      </c>
-      <c r="J96" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="K96" s="126" t="s">
-        <v>37</v>
-      </c>
-      <c r="L96" s="97" t="s">
-        <v>58</v>
-      </c>
-      <c r="M96" s="97" t="s">
-        <v>547</v>
-      </c>
-      <c r="N96" s="97" t="s">
-        <v>548</v>
-      </c>
-      <c r="O96" s="97" t="s">
-        <v>547</v>
-      </c>
-      <c r="P96" s="97" t="s">
-        <v>549</v>
-      </c>
-      <c r="Q96" s="97" t="s">
-        <v>414</v>
-      </c>
-      <c r="R96" s="97" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="55" customFormat="1" ht="28.8">
-      <c r="A97" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="B97" s="73" t="s">
-        <v>557</v>
-      </c>
-      <c r="C97" s="73"/>
-      <c r="D97" s="73" t="s">
-        <v>559</v>
-      </c>
-      <c r="E97" s="73" t="s">
-        <v>558</v>
-      </c>
-      <c r="F97" s="74">
-        <v>59.605499999999999</v>
-      </c>
-      <c r="G97" s="74">
-        <v>-151.4221</v>
-      </c>
-      <c r="H97" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="I97" s="76">
+      <c r="I97" s="75">
         <v>44035</v>
       </c>
       <c r="J97" s="41" t="s">
@@ -8224,26 +8209,26 @@
       <c r="K97" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="L97" s="73" t="s">
+      <c r="L97" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="M97" s="73" t="s">
+      <c r="M97" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="N97" s="73" t="s">
+      <c r="N97" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="O97" s="105" t="s">
+      <c r="O97" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="P97" s="110" t="s">
-        <v>553</v>
-      </c>
-      <c r="Q97" s="73" t="s">
+      <c r="P97" s="109" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q97" s="72" t="s">
         <v>414</v>
       </c>
-      <c r="R97" s="73" t="s">
-        <v>560</v>
+      <c r="R97" s="72" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="98" spans="1:18">
@@ -8252,7 +8237,7 @@
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
       <c r="E98" s="10"/>
-      <c r="H98" s="102"/>
+      <c r="H98" s="101"/>
       <c r="J98" s="23"/>
       <c r="K98" s="23"/>
       <c r="L98" s="10"/>
@@ -8262,28 +8247,6 @@
       <c r="P98" s="10"/>
       <c r="Q98" s="10"/>
       <c r="R98" s="10"/>
-    </row>
-    <row r="99" spans="1:18">
-      <c r="A99" s="50"/>
-      <c r="B99" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-    </row>
-    <row r="101" spans="1:18" ht="43.2">
-      <c r="A101" s="45"/>
-      <c r="B101" s="10" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" ht="187.2">
-      <c r="A103" s="49" t="s">
-        <v>536</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>567</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8307,7 +8270,7 @@
     <col min="18" max="18" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="72">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="57.6">
       <c r="A1" s="11" t="s">
         <v>282</v>
       </c>
@@ -8363,7 +8326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="62" customFormat="1" ht="72">
+    <row r="2" spans="1:19" s="61" customFormat="1" ht="72">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
@@ -8416,7 +8379,7 @@
       <c r="R2" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="S2" s="61"/>
+      <c r="S2" s="60"/>
     </row>
     <row r="3" spans="1:19" s="45" customFormat="1" ht="57.6">
       <c r="A3" s="10" t="s">
@@ -8469,7 +8432,7 @@
         <v>314</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S3" s="44"/>
     </row>
@@ -8526,10 +8489,10 @@
         <v>53</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>475</v>
-      </c>
-      <c r="S4" s="70" t="s">
-        <v>564</v>
+        <v>474</v>
+      </c>
+      <c r="S4" s="69" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="5" customFormat="1" ht="172.8">
@@ -8549,13 +8512,13 @@
       <c r="F5" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="70" t="s">
         <v>320</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="58" t="s">
         <v>321</v>
       </c>
       <c r="J5" s="23" t="s">
@@ -8583,211 +8546,211 @@
         <v>323</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="S5" s="42" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="91" customFormat="1" ht="345.6">
-      <c r="A6" s="89" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="90" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="90" customFormat="1" ht="345.6">
+      <c r="A6" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="89" t="s">
         <v>417</v>
       </c>
-      <c r="C6" s="91">
+      <c r="C6" s="90">
         <v>9455558</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="88" t="s">
         <v>424</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="F6" s="92">
+      <c r="F6" s="91">
         <v>59.602600000000002</v>
       </c>
-      <c r="G6" s="92">
+      <c r="G6" s="91">
         <v>-151.41030000000001</v>
       </c>
-      <c r="H6" s="93" t="s">
+      <c r="H6" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="94" t="s">
+      <c r="I6" s="93" t="s">
         <v>419</v>
       </c>
-      <c r="J6" s="95" t="s">
+      <c r="J6" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="95" t="s">
+      <c r="K6" s="94" t="s">
         <v>420</v>
       </c>
-      <c r="L6" s="89" t="s">
+      <c r="L6" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="89" t="s">
+      <c r="M6" s="88" t="s">
         <v>421</v>
       </c>
-      <c r="N6" s="89" t="s">
+      <c r="N6" s="88" t="s">
         <v>422</v>
       </c>
-      <c r="O6" s="89" t="s">
+      <c r="O6" s="88" t="s">
         <v>421</v>
       </c>
-      <c r="P6" s="89" t="s">
+      <c r="P6" s="88" t="s">
         <v>423</v>
       </c>
-      <c r="Q6" s="96" t="s">
+      <c r="Q6" s="95" t="s">
         <v>414</v>
       </c>
-      <c r="R6" s="89" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="91" customFormat="1" ht="86.4">
-      <c r="A7" s="91" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="118" t="s">
+      <c r="R6" s="88" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="90" customFormat="1" ht="86.4">
+      <c r="A7" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="117" t="s">
         <v>307</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="88" t="s">
         <v>438</v>
       </c>
-      <c r="E7" s="95" t="s">
+      <c r="E7" s="94" t="s">
         <v>439</v>
       </c>
-      <c r="F7" s="119">
+      <c r="F7" s="118">
         <v>55.315600000000003</v>
       </c>
-      <c r="G7" s="119">
+      <c r="G7" s="118">
         <v>-131.59379999999999</v>
       </c>
-      <c r="H7" s="119" t="s">
+      <c r="H7" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="120" t="s">
-        <v>519</v>
-      </c>
-      <c r="J7" s="95" t="s">
+      <c r="I7" s="119" t="s">
+        <v>517</v>
+      </c>
+      <c r="J7" s="94" t="s">
         <v>443</v>
       </c>
-      <c r="K7" s="119" t="s">
+      <c r="K7" s="118" t="s">
         <v>198</v>
       </c>
-      <c r="L7" s="119" t="s">
+      <c r="L7" s="118" t="s">
         <v>197</v>
       </c>
-      <c r="M7" s="119" t="s">
+      <c r="M7" s="118" t="s">
         <v>199</v>
       </c>
-      <c r="N7" s="119" t="s">
+      <c r="N7" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="119" t="s">
+      <c r="O7" s="118" t="s">
         <v>199</v>
       </c>
-      <c r="P7" s="119" t="s">
+      <c r="P7" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="Q7" s="119" t="s">
+      <c r="Q7" s="118" t="s">
         <v>346</v>
       </c>
-      <c r="R7" s="121"/>
-      <c r="S7" s="122" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="109" customFormat="1" ht="57.6">
-      <c r="A8" s="109" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="109" t="s">
+      <c r="R7" s="120"/>
+      <c r="S7" s="121" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="108" customFormat="1" ht="57.6">
+      <c r="A8" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="108" t="s">
+        <v>534</v>
+      </c>
+      <c r="D8" s="108" t="s">
+        <v>551</v>
+      </c>
+      <c r="H8" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="108">
+        <v>2019</v>
+      </c>
+      <c r="K8" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="L8" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="108" t="s">
+        <v>535</v>
+      </c>
+      <c r="N8" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="O8" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="P8" s="109" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q8" s="108" t="s">
         <v>537</v>
       </c>
-      <c r="D8" s="109" t="s">
-        <v>554</v>
-      </c>
-      <c r="H8" s="109" t="s">
+      <c r="R8" s="109" t="s">
+        <v>538</v>
+      </c>
+      <c r="S8" s="108" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="108" customFormat="1" ht="57.6">
+      <c r="A9" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="108" t="s">
+        <v>534</v>
+      </c>
+      <c r="D9" s="108" t="s">
+        <v>541</v>
+      </c>
+      <c r="H9" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="109">
+      <c r="I9" s="108">
         <v>2019</v>
       </c>
-      <c r="K8" s="109" t="s">
+      <c r="J9" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="108" t="s">
         <v>204</v>
       </c>
-      <c r="L8" s="109" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="109" t="s">
-        <v>538</v>
-      </c>
-      <c r="N8" s="109" t="s">
+      <c r="L9" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="109" t="s">
+        <v>535</v>
+      </c>
+      <c r="N9" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="O8" s="105" t="s">
+      <c r="O9" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="P8" s="110" t="s">
-        <v>539</v>
-      </c>
-      <c r="Q8" s="109" t="s">
-        <v>540</v>
-      </c>
-      <c r="R8" s="110" t="s">
-        <v>541</v>
-      </c>
-      <c r="S8" s="109" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="109" customFormat="1" ht="57.6">
-      <c r="A9" s="109" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="109" t="s">
+      <c r="P9" s="109" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q9" s="108" t="s">
         <v>537</v>
       </c>
-      <c r="D9" s="109" t="s">
-        <v>544</v>
-      </c>
-      <c r="H9" s="109" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="109">
-        <v>2019</v>
-      </c>
-      <c r="J9" s="109" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="109" t="s">
-        <v>204</v>
-      </c>
-      <c r="L9" s="109" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="110" t="s">
-        <v>538</v>
-      </c>
-      <c r="N9" s="109" t="s">
-        <v>206</v>
-      </c>
-      <c r="O9" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="P9" s="110" t="s">
-        <v>539</v>
-      </c>
-      <c r="Q9" s="109" t="s">
-        <v>540</v>
-      </c>
-      <c r="R9" s="110" t="s">
-        <v>545</v>
-      </c>
-      <c r="S9" s="109" t="s">
-        <v>563</v>
+      <c r="R9" s="109" t="s">
+        <v>542</v>
+      </c>
+      <c r="S9" s="108" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -8892,7 +8855,7 @@
         <v>224</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>225</v>
@@ -8936,61 +8899,61 @@
       <c r="S2" s="1"/>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:20" s="87" customFormat="1" ht="86.4">
-      <c r="A3" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="84" t="s">
+    <row r="3" spans="1:20" s="86" customFormat="1" ht="86.4">
+      <c r="A3" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="83" t="s">
         <v>217</v>
       </c>
-      <c r="F3" s="117" t="s">
+      <c r="F3" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="I3" s="86">
+      <c r="I3" s="85">
         <v>2008</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="84" t="s">
+      <c r="K3" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="84" t="s">
+      <c r="M3" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="N3" s="84" t="s">
+      <c r="N3" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="84" t="s">
+      <c r="O3" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="P3" s="84" t="s">
+      <c r="P3" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="Q3" s="85" t="s">
+      <c r="Q3" s="84" t="s">
         <v>222</v>
       </c>
-      <c r="R3" s="85" t="s">
+      <c r="R3" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="S3" s="84"/>
-      <c r="T3" s="88"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="87"/>
     </row>
     <row r="4" spans="1:20" s="3" customFormat="1" ht="86.4">
       <c r="A4" s="10" t="s">
@@ -9092,64 +9055,64 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="113" customFormat="1" ht="72">
+    <row r="7" spans="1:20" s="112" customFormat="1" ht="72">
       <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="113" t="s">
+      <c r="D7" s="112" t="s">
         <v>435</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="113" t="s">
         <v>425</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="113" t="s">
         <v>432</v>
       </c>
-      <c r="G7" s="113" t="s">
+      <c r="G7" s="112" t="s">
         <v>433</v>
       </c>
-      <c r="I7" s="115">
+      <c r="I7" s="114">
         <v>43040</v>
       </c>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="114" t="s">
+      <c r="K7" s="113" t="s">
         <v>426</v>
       </c>
-      <c r="L7" s="113" t="s">
+      <c r="L7" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="114" t="s">
+      <c r="M7" s="113" t="s">
         <v>427</v>
       </c>
-      <c r="N7" s="113" t="s">
+      <c r="N7" s="112" t="s">
         <v>428</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="P7" s="113" t="s">
+      <c r="P7" s="112" t="s">
         <v>430</v>
       </c>
-      <c r="Q7" s="114" t="s">
+      <c r="Q7" s="113" t="s">
         <v>431</v>
       </c>
-      <c r="R7" s="114" t="s">
+      <c r="R7" s="113" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="113" customFormat="1"/>
-    <row r="9" spans="1:20" s="113" customFormat="1"/>
-    <row r="10" spans="1:20" s="113" customFormat="1" ht="244.8">
-      <c r="A10" s="113" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="114" t="s">
-        <v>463</v>
+    <row r="8" spans="1:20" s="112" customFormat="1"/>
+    <row r="9" spans="1:20" s="112" customFormat="1"/>
+    <row r="10" spans="1:20" s="112" customFormat="1" ht="244.8">
+      <c r="A10" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>462</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>218</v>
@@ -9157,39 +9120,39 @@
       <c r="G10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="113" t="s">
+      <c r="H10" s="112" t="s">
         <v>200</v>
       </c>
-      <c r="I10" s="116">
+      <c r="I10" s="115">
         <v>43282</v>
       </c>
-      <c r="J10" s="113" t="s">
+      <c r="J10" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="113" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="113" t="s">
+      <c r="K10" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="114" t="s">
+      <c r="M10" s="113" t="s">
+        <v>458</v>
+      </c>
+      <c r="N10" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="112" t="s">
         <v>459</v>
       </c>
-      <c r="N10" s="113" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" s="113" t="s">
-        <v>460</v>
-      </c>
-      <c r="P10" s="113" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="52" t="s">
-        <v>562</v>
+      <c r="P10" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="51" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="51"/>
+      <c r="A13" s="50"/>
       <c r="B13" t="s">
         <v>442</v>
       </c>

</xml_diff>

<commit_message>
fixed coords for juneau library and salmon landing
</commit_message>
<xml_diff>
--- a/2020/data/processed/AOOS.xlsx
+++ b/2020/data/processed/AOOS.xlsx
@@ -2907,9 +2907,9 @@
   <dimension ref="A1:T98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4475,7 +4475,7 @@
         <v>122</v>
       </c>
       <c r="F29" s="31">
-        <v>28.298233</v>
+        <v>58.298233000000003</v>
       </c>
       <c r="G29" s="31">
         <v>-134.404517</v>

</xml_diff>

<commit_message>
cleaning extra lines and columns.
</commit_message>
<xml_diff>
--- a/2020/data/processed/AOOS.xlsx
+++ b/2020/data/processed/AOOS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="566">
   <si>
     <t>Station ID</t>
   </si>
@@ -1308,9 +1308,6 @@
   </si>
   <si>
     <t>TKEA2 </t>
-  </si>
-  <si>
-    <t>New</t>
   </si>
   <si>
     <r>
@@ -1841,13 +1838,7 @@
     <t>1/23/2009; 05/05/15</t>
   </si>
   <si>
-    <t>Stopped reporting in February 2020; I am told this Kotzebue stations i essentially the same station as KZTA2. The yellow one is a redeployed version that reported in 2020…but has not been properly assigned the CMAN with River forecast office. Duplicate station pages resolved in 2020.</t>
-  </si>
-  <si>
     <t>Kotzebue Sound at Kotzebue</t>
-  </si>
-  <si>
-    <t>Stopped reportng July 2020.</t>
   </si>
   <si>
     <t>NREL Kodiak, AK CDIP Wave Buoy 236</t>
@@ -2906,10 +2897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3039,10 +3030,10 @@
         <v>37</v>
       </c>
       <c r="Q2" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S2" s="1"/>
     </row>
@@ -3051,14 +3042,14 @@
         <v>37</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F3" s="22">
         <v>59.014200000000002</v>
@@ -3067,7 +3058,7 @@
         <v>-148.6902</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I3" s="2">
         <v>43657</v>
@@ -3076,7 +3067,7 @@
         <v>35</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>36</v>
@@ -3094,10 +3085,10 @@
         <v>37</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="72">
@@ -3105,16 +3096,16 @@
         <v>37</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F4" s="29">
         <v>59.016500000000001</v>
@@ -3123,7 +3114,7 @@
         <v>-148.696</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I4" s="2">
         <v>43657</v>
@@ -3132,7 +3123,7 @@
         <v>35</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>36</v>
@@ -3150,10 +3141,10 @@
         <v>37</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="57.6">
@@ -3204,7 +3195,7 @@
         <v>79</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>80</v>
@@ -3253,7 +3244,7 @@
         <v>67</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>68</v>
@@ -3305,7 +3296,7 @@
         <v>67</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>68</v>
@@ -3321,7 +3312,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>155</v>
@@ -3427,14 +3418,14 @@
         <v>37</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="40" t="s">
+        <v>494</v>
+      </c>
+      <c r="E10" s="40" t="s">
         <v>495</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>496</v>
       </c>
       <c r="F10" s="77">
         <v>60.791499999999999</v>
@@ -3473,7 +3464,7 @@
         <v>314</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="S10" s="47"/>
     </row>
@@ -3530,7 +3521,7 @@
         <v>314</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -3542,7 +3533,7 @@
         <v>329</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>288</v>
@@ -3745,11 +3736,11 @@
         <v>37</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="46" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>347</v>
@@ -3770,7 +3761,7 @@
         <v>35</v>
       </c>
       <c r="K16" s="40" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L16" s="46" t="s">
         <v>36</v>
@@ -3788,10 +3779,10 @@
         <v>37</v>
       </c>
       <c r="Q16" s="97" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="R16" s="46" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="28.8">
@@ -3907,14 +3898,14 @@
         <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F19" s="29">
         <v>63.776913</v>
@@ -3932,7 +3923,7 @@
         <v>35</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>36</v>
@@ -3958,14 +3949,14 @@
         <v>37</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F20" s="77">
         <v>58.211799999999997</v>
@@ -4004,7 +3995,7 @@
         <v>314</v>
       </c>
       <c r="R20" s="40" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="S20" s="47"/>
     </row>
@@ -4116,7 +4107,7 @@
         <v>314</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="S22" s="35"/>
     </row>
@@ -4565,7 +4556,7 @@
         <v>314</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="28.8">
@@ -5454,7 +5445,7 @@
         <v>37</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C47" s="98" t="s">
         <v>371</v>
@@ -5499,10 +5490,10 @@
         <v>283</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="28.8">
@@ -5565,14 +5556,14 @@
         <v>37</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="E49" s="10" t="s">
         <v>399</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>400</v>
       </c>
       <c r="F49" s="29">
         <v>63.692644999999999</v>
@@ -5590,7 +5581,7 @@
         <v>35</v>
       </c>
       <c r="K49" s="23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>36</v>
@@ -5611,7 +5602,7 @@
         <v>314</v>
       </c>
       <c r="R49" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="28.8">
@@ -5728,14 +5719,14 @@
         <v>37</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C52" s="46"/>
       <c r="D52" s="46" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E52" s="72" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F52" s="65">
         <v>53.5989</v>
@@ -5753,7 +5744,7 @@
         <v>35</v>
       </c>
       <c r="K52" s="40" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L52" s="46" t="s">
         <v>36</v>
@@ -5771,10 +5762,10 @@
         <v>37</v>
       </c>
       <c r="Q52" s="97" t="s">
+        <v>490</v>
+      </c>
+      <c r="R52" s="46" t="s">
         <v>491</v>
-      </c>
-      <c r="R52" s="46" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="53" spans="1:20" s="32" customFormat="1" ht="28.8">
@@ -5902,7 +5893,7 @@
         <v>356</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E55" s="31" t="s">
         <v>122</v>
@@ -6010,14 +6001,14 @@
         <v>37</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C57" s="80"/>
       <c r="D57" s="78" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E57" s="72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F57" s="79">
         <v>54.802599999999998</v>
@@ -6054,7 +6045,7 @@
         <v>314</v>
       </c>
       <c r="R57" s="78" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="S57" s="81"/>
     </row>
@@ -6066,7 +6057,7 @@
         <v>144</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>92</v>
@@ -6234,7 +6225,7 @@
         <v>84</v>
       </c>
       <c r="I61" s="59" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>35</v>
@@ -6326,7 +6317,7 @@
         <v>46108</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>312</v>
@@ -6347,7 +6338,7 @@
         <v>35</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L63" s="40" t="s">
         <v>197</v>
@@ -6368,7 +6359,7 @@
         <v>313</v>
       </c>
       <c r="R63" s="43" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T63" s="5"/>
     </row>
@@ -6377,13 +6368,13 @@
         <v>59</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C64" s="10">
         <v>46264</v>
       </c>
       <c r="D64" s="46" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>310</v>
@@ -6404,7 +6395,7 @@
         <v>35</v>
       </c>
       <c r="K64" s="23" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>36</v>
@@ -6422,10 +6413,10 @@
         <v>40</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="R64" s="40" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="65" spans="1:20" s="19" customFormat="1" ht="125.25" customHeight="1">
@@ -6439,10 +6430,10 @@
         <v>46265</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F65" s="1">
         <v>64.472300000000004</v>
@@ -6457,10 +6448,10 @@
         <v>43297</v>
       </c>
       <c r="J65" s="40" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>36</v>
@@ -6478,10 +6469,10 @@
         <v>40</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="R65" s="40" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="S65" s="3"/>
       <c r="T65" s="5"/>
@@ -6749,7 +6740,7 @@
         <v>178</v>
       </c>
       <c r="Q70" s="31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R70" s="37" t="s">
         <v>345</v>
@@ -6764,7 +6755,7 @@
         <v>185</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>186</v>
@@ -6818,7 +6809,7 @@
         <v>308</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>192</v>
@@ -6860,24 +6851,22 @@
         <v>346</v>
       </c>
       <c r="R72" s="40" t="s">
-        <v>516</v>
-      </c>
-      <c r="S72" s="3" t="s">
-        <v>382</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="S72" s="3"/>
     </row>
     <row r="73" spans="1:20" s="49" customFormat="1" ht="43.2">
       <c r="A73" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B73" s="63" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D73" s="46" t="s">
+        <v>516</v>
+      </c>
+      <c r="E73" s="40" t="s">
         <v>519</v>
-      </c>
-      <c r="E73" s="40" t="s">
-        <v>522</v>
       </c>
       <c r="F73" s="47">
         <v>50.116</v>
@@ -6895,7 +6884,7 @@
         <v>35</v>
       </c>
       <c r="K73" s="40" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L73" s="40" t="s">
         <v>77</v>
@@ -6904,7 +6893,7 @@
         <v>199</v>
       </c>
       <c r="N73" s="40" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="O73" s="40" t="s">
         <v>199</v>
@@ -6916,7 +6905,7 @@
         <v>346</v>
       </c>
       <c r="R73" s="40" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="S73" s="105"/>
     </row>
@@ -6967,7 +6956,7 @@
         <v>207</v>
       </c>
       <c r="P74" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q74" s="21" t="s">
         <v>338</v>
@@ -6981,14 +6970,14 @@
         <v>37</v>
       </c>
       <c r="B75" s="68" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C75" s="72"/>
       <c r="D75" s="41" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E75" s="64" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F75" s="57">
         <v>66.895034999999993</v>
@@ -7003,7 +6992,7 @@
         <v>43348</v>
       </c>
       <c r="J75" s="64" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K75" s="64" t="s">
         <v>204</v>
@@ -7021,16 +7010,13 @@
         <v>207</v>
       </c>
       <c r="P75" s="64" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q75" s="107" t="s">
         <v>338</v>
       </c>
       <c r="R75" s="64" t="s">
-        <v>467</v>
-      </c>
-      <c r="S75" s="54" t="s">
-        <v>506</v>
+        <v>466</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="28.8">
@@ -7044,10 +7030,10 @@
         <v>373</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F76" s="1">
         <v>66.926820000000006</v>
@@ -7062,7 +7048,7 @@
         <v>42269</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>204</v>
@@ -7080,7 +7066,7 @@
         <v>207</v>
       </c>
       <c r="P76" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q76" s="21" t="s">
         <v>338</v>
@@ -7088,9 +7074,7 @@
       <c r="R76" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="S76" s="19" t="s">
-        <v>508</v>
-      </c>
+      <c r="S76" s="19"/>
       <c r="T76" s="19"/>
     </row>
     <row r="77" spans="1:20">
@@ -7138,7 +7122,7 @@
         <v>207</v>
       </c>
       <c r="P77" s="40" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q77" s="21" t="s">
         <v>338</v>
@@ -7759,11 +7743,11 @@
         <v>37</v>
       </c>
       <c r="B89" s="54" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C89" s="66"/>
       <c r="D89" s="66" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E89" s="66" t="s">
         <v>348</v>
@@ -7775,7 +7759,7 @@
         <v>-147.70140000000001</v>
       </c>
       <c r="H89" s="67" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I89" s="56">
         <v>43307</v>
@@ -7790,22 +7774,22 @@
         <v>77</v>
       </c>
       <c r="M89" s="66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N89" s="66" t="s">
         <v>46</v>
       </c>
       <c r="O89" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="P89" s="66" t="s">
         <v>450</v>
-      </c>
-      <c r="P89" s="66" t="s">
-        <v>451</v>
       </c>
       <c r="Q89" s="57" t="s">
         <v>314</v>
       </c>
       <c r="R89" s="72" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="90" spans="1:19" ht="57.6">
@@ -7813,14 +7797,14 @@
         <v>37</v>
       </c>
       <c r="B90" s="54" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C90" s="66"/>
       <c r="D90" s="66" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E90" s="76" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F90" s="55">
         <v>70.319000000000003</v>
@@ -7829,13 +7813,13 @@
         <v>-147.7612</v>
       </c>
       <c r="H90" s="67" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I90" s="56">
         <v>43683</v>
       </c>
       <c r="J90" s="41" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K90" s="64" t="s">
         <v>266</v>
@@ -7844,22 +7828,22 @@
         <v>77</v>
       </c>
       <c r="M90" s="66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N90" s="66" t="s">
         <v>46</v>
       </c>
       <c r="O90" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="P90" s="66" t="s">
         <v>450</v>
       </c>
-      <c r="P90" s="66" t="s">
-        <v>451</v>
-      </c>
       <c r="Q90" s="66" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R90" s="72" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="91" spans="1:19" ht="57.6">
@@ -7867,14 +7851,14 @@
         <v>37</v>
       </c>
       <c r="B91" s="54" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C91" s="66"/>
       <c r="D91" s="66" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E91" s="76" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F91" s="55">
         <v>70.393500000000003</v>
@@ -7883,13 +7867,13 @@
         <v>-147.83500000000001</v>
       </c>
       <c r="H91" s="67" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I91" s="56">
         <v>43684</v>
       </c>
       <c r="J91" s="41" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K91" s="64" t="s">
         <v>266</v>
@@ -7898,22 +7882,22 @@
         <v>77</v>
       </c>
       <c r="M91" s="66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N91" s="66" t="s">
         <v>46</v>
       </c>
       <c r="O91" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="P91" s="66" t="s">
         <v>450</v>
       </c>
-      <c r="P91" s="66" t="s">
-        <v>451</v>
-      </c>
       <c r="Q91" s="66" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R91" s="72" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="92" spans="1:19" s="76" customFormat="1" ht="43.2">
@@ -7921,13 +7905,13 @@
         <v>37</v>
       </c>
       <c r="B92" s="72" t="s">
+        <v>475</v>
+      </c>
+      <c r="D92" s="72" t="s">
         <v>476</v>
       </c>
-      <c r="D92" s="72" t="s">
-        <v>477</v>
-      </c>
       <c r="E92" s="72" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F92" s="73">
         <v>59.798299999999998</v>
@@ -7945,25 +7929,25 @@
         <v>35</v>
       </c>
       <c r="K92" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L92" s="72" t="s">
         <v>77</v>
       </c>
       <c r="M92" s="72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N92" s="72" t="s">
         <v>38</v>
       </c>
       <c r="O92" s="72" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="P92" s="72" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="Q92" s="72" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="93" spans="1:19" s="76" customFormat="1" ht="100.8">
@@ -7971,13 +7955,13 @@
         <v>37</v>
       </c>
       <c r="B93" s="72" t="s">
+        <v>480</v>
+      </c>
+      <c r="D93" s="72" t="s">
         <v>481</v>
       </c>
-      <c r="D93" s="72" t="s">
-        <v>482</v>
-      </c>
       <c r="E93" s="72" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F93" s="73">
         <v>61.091000000000001</v>
@@ -7986,7 +7970,7 @@
         <v>-146.3766</v>
       </c>
       <c r="H93" s="74" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I93" s="75">
         <v>43729</v>
@@ -7995,28 +7979,28 @@
         <v>35</v>
       </c>
       <c r="K93" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L93" s="72" t="s">
         <v>77</v>
       </c>
       <c r="M93" s="72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N93" s="72" t="s">
         <v>38</v>
       </c>
       <c r="O93" s="72" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="P93" s="72" t="s">
         <v>245</v>
       </c>
       <c r="Q93" s="72" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="R93" s="72" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="1:19" s="76" customFormat="1" ht="100.8">
@@ -8024,13 +8008,13 @@
         <v>37</v>
       </c>
       <c r="B94" s="72" t="s">
+        <v>483</v>
+      </c>
+      <c r="D94" s="72" t="s">
         <v>484</v>
       </c>
-      <c r="D94" s="72" t="s">
+      <c r="E94" s="72" t="s">
         <v>485</v>
-      </c>
-      <c r="E94" s="72" t="s">
-        <v>486</v>
       </c>
       <c r="F94" s="73">
         <v>61.122500000000002</v>
@@ -8039,7 +8023,7 @@
         <v>-146.29669999999999</v>
       </c>
       <c r="H94" s="74" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I94" s="75">
         <v>43729</v>
@@ -8048,28 +8032,28 @@
         <v>35</v>
       </c>
       <c r="K94" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L94" s="72" t="s">
         <v>77</v>
       </c>
       <c r="M94" s="72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N94" s="72" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="O94" s="72" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="P94" s="72" t="s">
         <v>245</v>
       </c>
       <c r="Q94" s="72" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="R94" s="72" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="95" spans="1:19" s="108" customFormat="1">
@@ -8077,13 +8061,13 @@
         <v>37</v>
       </c>
       <c r="B95" s="108" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D95" s="108" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E95" s="108" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F95" s="111">
         <v>56.004100000000001</v>
@@ -8101,7 +8085,7 @@
         <v>35</v>
       </c>
       <c r="K95" s="109" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L95" s="108" t="s">
         <v>77</v>
@@ -8116,10 +8100,10 @@
         <v>207</v>
       </c>
       <c r="P95" s="109" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="Q95" s="108" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R95" s="109"/>
     </row>
@@ -8128,14 +8112,14 @@
         <v>37</v>
       </c>
       <c r="B96" s="96" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C96" s="96"/>
       <c r="D96" s="96" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E96" s="96" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F96" s="122">
         <v>58.732100000000003</v>
@@ -8159,22 +8143,22 @@
         <v>58</v>
       </c>
       <c r="M96" s="96" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N96" s="96" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="O96" s="96" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P96" s="96" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="Q96" s="96" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R96" s="96" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="97" spans="1:18" s="54" customFormat="1" ht="28.8">
@@ -8182,14 +8166,14 @@
         <v>37</v>
       </c>
       <c r="B97" s="72" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C97" s="72"/>
       <c r="D97" s="72" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E97" s="72" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F97" s="73">
         <v>59.605499999999999</v>
@@ -8222,13 +8206,13 @@
         <v>207</v>
       </c>
       <c r="P97" s="109" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="Q97" s="72" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R97" s="72" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="98" spans="1:18">
@@ -8432,7 +8416,7 @@
         <v>314</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="S3" s="44"/>
     </row>
@@ -8465,7 +8449,7 @@
         <v>42253</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>52</v>
@@ -8489,10 +8473,10 @@
         <v>53</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="S4" s="69" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="5" customFormat="1" ht="172.8">
@@ -8546,10 +8530,10 @@
         <v>323</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="S5" s="42" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="90" customFormat="1" ht="345.6">
@@ -8557,16 +8541,16 @@
         <v>37</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C6" s="90">
         <v>9455558</v>
       </c>
       <c r="D6" s="88" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F6" s="91">
         <v>59.602600000000002</v>
@@ -8578,34 +8562,34 @@
         <v>84</v>
       </c>
       <c r="I6" s="93" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J6" s="94" t="s">
         <v>77</v>
       </c>
       <c r="K6" s="94" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L6" s="88" t="s">
         <v>77</v>
       </c>
       <c r="M6" s="88" t="s">
+        <v>420</v>
+      </c>
+      <c r="N6" s="88" t="s">
         <v>421</v>
       </c>
-      <c r="N6" s="88" t="s">
+      <c r="O6" s="88" t="s">
+        <v>420</v>
+      </c>
+      <c r="P6" s="88" t="s">
         <v>422</v>
       </c>
-      <c r="O6" s="88" t="s">
-        <v>421</v>
-      </c>
-      <c r="P6" s="88" t="s">
-        <v>423</v>
-      </c>
       <c r="Q6" s="95" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R6" s="88" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="90" customFormat="1" ht="86.4">
@@ -8616,10 +8600,10 @@
         <v>307</v>
       </c>
       <c r="D7" s="88" t="s">
+        <v>437</v>
+      </c>
+      <c r="E7" s="94" t="s">
         <v>438</v>
-      </c>
-      <c r="E7" s="94" t="s">
-        <v>439</v>
       </c>
       <c r="F7" s="118">
         <v>55.315600000000003</v>
@@ -8631,10 +8615,10 @@
         <v>84</v>
       </c>
       <c r="I7" s="119" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="J7" s="94" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K7" s="118" t="s">
         <v>198</v>
@@ -8659,7 +8643,7 @@
       </c>
       <c r="R7" s="120"/>
       <c r="S7" s="121" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="108" customFormat="1" ht="57.6">
@@ -8667,10 +8651,10 @@
         <v>37</v>
       </c>
       <c r="B8" s="108" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D8" s="108" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H8" s="108" t="s">
         <v>84</v>
@@ -8685,7 +8669,7 @@
         <v>36</v>
       </c>
       <c r="M8" s="108" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="N8" s="108" t="s">
         <v>206</v>
@@ -8694,16 +8678,16 @@
         <v>207</v>
       </c>
       <c r="P8" s="109" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="Q8" s="108" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="R8" s="109" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="S8" s="108" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="108" customFormat="1" ht="57.6">
@@ -8711,10 +8695,10 @@
         <v>37</v>
       </c>
       <c r="B9" s="108" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D9" s="108" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H9" s="108" t="s">
         <v>84</v>
@@ -8732,7 +8716,7 @@
         <v>35</v>
       </c>
       <c r="M9" s="109" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="N9" s="108" t="s">
         <v>206</v>
@@ -8741,16 +8725,16 @@
         <v>207</v>
       </c>
       <c r="P9" s="109" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="Q9" s="108" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="R9" s="109" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="S9" s="108" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -8855,7 +8839,7 @@
         <v>224</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>225</v>
@@ -8950,7 +8934,7 @@
         <v>222</v>
       </c>
       <c r="R3" s="84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S3" s="83"/>
       <c r="T3" s="87"/>
@@ -9060,16 +9044,16 @@
         <v>37</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E7" s="113" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F7" s="113" t="s">
+        <v>431</v>
+      </c>
+      <c r="G7" s="112" t="s">
         <v>432</v>
-      </c>
-      <c r="G7" s="112" t="s">
-        <v>433</v>
       </c>
       <c r="I7" s="114">
         <v>43040</v>
@@ -9078,28 +9062,28 @@
         <v>35</v>
       </c>
       <c r="K7" s="113" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L7" s="112" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="113" t="s">
+        <v>426</v>
+      </c>
+      <c r="N7" s="112" t="s">
         <v>427</v>
       </c>
-      <c r="N7" s="112" t="s">
+      <c r="O7" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="112" t="s">
         <v>429</v>
       </c>
-      <c r="P7" s="112" t="s">
+      <c r="Q7" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="Q7" s="113" t="s">
-        <v>431</v>
-      </c>
       <c r="R7" s="113" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="112" customFormat="1"/>
@@ -9109,10 +9093,10 @@
         <v>37</v>
       </c>
       <c r="B10" s="113" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>218</v>
@@ -9136,25 +9120,25 @@
         <v>58</v>
       </c>
       <c r="M10" s="113" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="N10" s="112" t="s">
         <v>46</v>
       </c>
       <c r="O10" s="112" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P10" s="112" t="s">
         <v>37</v>
       </c>
       <c r="Q10" s="51" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="50"/>
       <c r="B13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>